<commit_message>
style: result page and upload page style changed
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +49,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -415,11 +414,14 @@
   </sheetPr>
   <dimension ref="A1:A42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="23.109375" customWidth="1" min="1" max="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -440,7 +442,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">| HR260K63379m
+          <t xml:space="preserve">Pr BH O01 AA
 </t>
         </is>
       </c>
@@ -448,7 +450,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">www alamy
+          <t xml:space="preserve">W720 BOM
 </t>
         </is>
       </c>
@@ -456,7 +458,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve">ee
+          <t xml:space="preserve">| HR260K63379m
 </t>
         </is>
       </c>
@@ -464,7 +466,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">“Mercedes
+          <t xml:space="preserve">~ TT
 </t>
         </is>
       </c>
@@ -472,7 +474,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">West co.uk
+          <t xml:space="preserve">Team.
 </t>
         </is>
       </c>
@@ -480,7 +482,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">“Benz Souil
+          <t xml:space="preserve">TANTZ DE A33]
 </t>
         </is>
       </c>
@@ -488,7 +490,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve">ee
+          <t xml:space="preserve">| HR260K63379m
 </t>
         </is>
       </c>
@@ -496,7 +498,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Team.
+          <t xml:space="preserve">www alamy
 </t>
         </is>
       </c>
@@ -504,7 +506,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve">TANTZ DE A33]
+          <t xml:space="preserve">“Mercedes
 </t>
         </is>
       </c>
@@ -512,7 +514,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve">W720 BOM
+          <t xml:space="preserve">ee
 </t>
         </is>
       </c>
@@ -520,7 +522,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve">W720 BOM
+          <t xml:space="preserve">West co.uk
 </t>
         </is>
       </c>
@@ -528,7 +530,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve">W720 BOM
+          <t xml:space="preserve">“Benz Souil
 </t>
         </is>
       </c>
@@ -536,7 +538,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t xml:space="preserve">www alamy
+          <t xml:space="preserve">ee
 </t>
         </is>
       </c>
@@ -544,7 +546,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t xml:space="preserve">ee
+          <t xml:space="preserve">www alamy
 </t>
         </is>
       </c>
@@ -552,7 +554,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve">“Mercedes
+          <t xml:space="preserve">ee
 </t>
         </is>
       </c>
@@ -560,7 +562,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t xml:space="preserve">West co.uk
+          <t xml:space="preserve">ee
 </t>
         </is>
       </c>
@@ -568,7 +570,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t xml:space="preserve">“Benz Souil
+          <t xml:space="preserve">“Mercedes
 </t>
         </is>
       </c>
@@ -576,7 +578,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t xml:space="preserve">ee
+          <t xml:space="preserve">West co.uk
 </t>
         </is>
       </c>
@@ -584,7 +586,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t xml:space="preserve">| HR260K63379m
+          <t xml:space="preserve">“Benz Souil
 </t>
         </is>
       </c>
@@ -592,7 +594,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t xml:space="preserve">W720 BOM
+          <t xml:space="preserve">www alamy
 </t>
         </is>
       </c>
@@ -600,7 +602,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t xml:space="preserve">| HR260K63379m
+          <t xml:space="preserve">ee
 </t>
         </is>
       </c>
@@ -608,7 +610,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t xml:space="preserve">www alamy
+          <t xml:space="preserve">ee
 </t>
         </is>
       </c>
@@ -616,7 +618,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t xml:space="preserve">ee
+          <t xml:space="preserve">“Mercedes
 </t>
         </is>
       </c>
@@ -624,7 +626,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t xml:space="preserve">ee
+          <t xml:space="preserve">West co.uk
 </t>
         </is>
       </c>
@@ -632,7 +634,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t xml:space="preserve">“Mercedes
+          <t xml:space="preserve">“Benz Souil
 </t>
         </is>
       </c>
@@ -640,7 +642,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t xml:space="preserve">West co.uk
+          <t xml:space="preserve">ee
 </t>
         </is>
       </c>
@@ -648,7 +650,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t xml:space="preserve">“Benz Souil
+          <t xml:space="preserve">“Mercedes
 </t>
         </is>
       </c>
@@ -656,7 +658,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t xml:space="preserve">www alamy
+          <t xml:space="preserve">West co.uk
 </t>
         </is>
       </c>
@@ -664,7 +666,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t xml:space="preserve">ee
+          <t xml:space="preserve">“Benz Souil
 </t>
         </is>
       </c>
@@ -680,7 +682,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t xml:space="preserve">“Mercedes
+          <t xml:space="preserve">www alamy
 </t>
         </is>
       </c>
@@ -688,7 +690,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t xml:space="preserve">West co.uk
+          <t xml:space="preserve">ee
 </t>
         </is>
       </c>
@@ -696,7 +698,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t xml:space="preserve">“Benz Souil
+          <t xml:space="preserve">“Mercedes
 </t>
         </is>
       </c>
@@ -704,7 +706,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t xml:space="preserve">| HR260K63379m
+          <t xml:space="preserve">West co.uk
 </t>
         </is>
       </c>
@@ -712,7 +714,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t xml:space="preserve">W720 BOM
+          <t xml:space="preserve">“Benz Souil
 </t>
         </is>
       </c>
@@ -720,7 +722,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t xml:space="preserve">| HR260K63379m
+          <t xml:space="preserve">ee
 </t>
         </is>
       </c>
@@ -728,7 +730,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t xml:space="preserve">| HR260K63379m
+          <t xml:space="preserve">www alamy
 </t>
         </is>
       </c>
@@ -736,7 +738,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Team.
+          <t xml:space="preserve">Pr BH O01 AA
 </t>
         </is>
       </c>
@@ -744,7 +746,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t xml:space="preserve">TANTZ DE A33]
+          <t xml:space="preserve">| HR260K63379m
 </t>
         </is>
       </c>
@@ -752,7 +754,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pr BH O01 AA
+          <t xml:space="preserve">| HR260K63379m
 </t>
         </is>
       </c>

</xml_diff>

<commit_message>
feat: updated some changes
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A42"/>
+  <dimension ref="A1:A44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -759,6 +759,22 @@
         </is>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">| HR260K63379m
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">W720 BOM
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>